<commit_message>
implemented modifications to warn if more than one run_parameters table is found, added to tests, did not update assertion yet
</commit_message>
<xml_diff>
--- a/adapter/tests/test1.xlsx
+++ b/adapter/tests/test1.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mg\code\repos\adapter\adapter\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrahovac/repos/adapter/adapter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1DB3CE-668F-413D-B560-7F2FF8AD0F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D28C04-C6DF-664C-84CD-3DF27FEFB0F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51636" yWindow="6552" windowWidth="28776" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4060" yWindow="4140" windowWidth="20780" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
+    <sheet name="test1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>a</t>
   </si>
@@ -56,6 +56,21 @@
   </si>
   <si>
     <t>cc</t>
+  </si>
+  <si>
+    <t>Duplicate run_parameters table</t>
+  </si>
+  <si>
+    <t>Output Path</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>vTest</t>
   </si>
 </sst>
 </file>
@@ -539,8 +554,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -620,6 +636,17 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="col_33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{604C90E3-9BB0-5E45-858B-22E37D8B46C9}" name="run_parameters30" displayName="run_parameters30" ref="F2:G3" totalsRowShown="0">
+  <autoFilter ref="F2:G3" xr:uid="{BC22F1F9-761A-A24E-AD17-6018D7D8BDCD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{04C727FD-CF1E-C446-812B-B19C9A8E618F}" name="Output Path"/>
+    <tableColumn id="2" xr3:uid="{698E1E68-EB01-8644-BF42-3F7A44C329EA}" name="Version"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -886,15 +913,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -904,8 +936,14 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -915,8 +953,14 @@
       <c r="D3">
         <v>12</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -927,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>1</v>
       </c>
@@ -938,7 +982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -949,7 +993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>11</v>
       </c>
@@ -960,7 +1004,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>11</v>
       </c>
@@ -971,7 +1015,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>11</v>
       </c>
@@ -984,9 +1028,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>